<commit_message>
p4a shell program started
</commit_message>
<xml_diff>
--- a/2.3-SE-4348.502-OS/Project4a/Burndown Chart.xlsx
+++ b/2.3-SE-4348.502-OS/Project4a/Burndown Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Screen-Cleaner\GitHub\UTDFall2018\2.3-SE-4348.502-OS\Project4a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9721DBC1-2205-4081-9F5D-D94333DC4EB2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94702902-B416-42FB-938F-9EB8489E4E31}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -619,7 +619,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -708,22 +708,22 @@
                   <c:v>-0.89999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.89999999999999991</c:v>
+                  <c:v>-1.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.89999999999999991</c:v>
+                  <c:v>-1.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.89999999999999991</c:v>
+                  <c:v>-1.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.89999999999999991</c:v>
+                  <c:v>-1.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.89999999999999991</c:v>
+                  <c:v>-1.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.89999999999999991</c:v>
+                  <c:v>-1.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2046,8 +2046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AK62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="F7" s="2">
         <f t="shared" ref="F7:F15" si="2">SUM(H7:R7)</f>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="G7" s="10">
         <v>1</v>
@@ -2265,7 +2265,9 @@
       <c r="J7" s="2"/>
       <c r="K7" s="11"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="M7" s="2">
+        <v>0.1</v>
+      </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -2284,7 +2286,7 @@
       </c>
       <c r="F8" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G8" s="10">
         <v>0</v>
@@ -2294,7 +2296,9 @@
       <c r="J8" s="2"/>
       <c r="K8" s="11"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="M8" s="2">
+        <v>0.1</v>
+      </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
@@ -2343,7 +2347,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="2">
@@ -2371,7 +2375,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G11" s="10">
         <v>0</v>
@@ -2381,7 +2385,9 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="M11" s="2">
+        <v>0.1</v>
+      </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
@@ -2917,7 +2923,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1">
         <f>G35-SUM(G9:G25)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
@@ -2980,7 +2986,7 @@
       </c>
       <c r="M37" s="23">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="N37" s="23">
         <f t="shared" si="4"/>
@@ -3053,27 +3059,27 @@
       </c>
       <c r="M38" s="23">
         <f t="shared" si="5"/>
-        <v>-0.89999999999999991</v>
+        <v>-1.2</v>
       </c>
       <c r="N38" s="23">
         <f t="shared" si="5"/>
-        <v>-0.89999999999999991</v>
+        <v>-1.2</v>
       </c>
       <c r="O38" s="23">
         <f t="shared" si="5"/>
-        <v>-0.89999999999999991</v>
+        <v>-1.2</v>
       </c>
       <c r="P38" s="23">
         <f t="shared" si="5"/>
-        <v>-0.89999999999999991</v>
+        <v>-1.2</v>
       </c>
       <c r="Q38" s="23">
         <f t="shared" si="5"/>
-        <v>-0.89999999999999991</v>
+        <v>-1.2</v>
       </c>
       <c r="R38" s="23">
         <f t="shared" si="5"/>
-        <v>-0.89999999999999991</v>
+        <v>-1.2</v>
       </c>
       <c r="S38" s="23"/>
       <c r="T38" s="23"/>

</xml_diff>